<commit_message>
Ne and peak fit error prop
</commit_message>
<xml_diff>
--- a/docs/Examples/Example1c_HORIBA_Calibration/PseudoVoigt.xlsx
+++ b/docs/Examples/Example1c_HORIBA_Calibration/PseudoVoigt.xlsx
@@ -807,55 +807,55 @@
         <v>33</v>
       </c>
       <c r="C2">
-        <v>1.001156862661844</v>
+        <v>1.001156862686675</v>
       </c>
       <c r="D2">
-        <v>330.0957588883418</v>
+        <v>330.0957588801548</v>
       </c>
       <c r="E2">
-        <v>1447.744338428079</v>
+        <v>1447.744338421631</v>
       </c>
       <c r="F2">
-        <v>1117.648579539737</v>
+        <v>1117.648579541477</v>
       </c>
       <c r="G2">
-        <v>215902.7009288698</v>
+        <v>215902.7063533315</v>
       </c>
       <c r="H2">
-        <v>46564.9046433331</v>
+        <v>46564.90486288338</v>
       </c>
       <c r="I2">
-        <v>2838.931105581772</v>
+        <v>2838.930856420813</v>
       </c>
       <c r="J2">
-        <v>207.4016139884059</v>
+        <v>207.4016431418981</v>
       </c>
       <c r="K2">
-        <v>1.353410252465042</v>
+        <v>1.353410308273159</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>0.09669999999999999</v>
       </c>
       <c r="N2">
-        <v>1.485888190266849E-09</v>
+        <v>1.4860370156633E-09</v>
       </c>
       <c r="O2">
-        <v>1.162331196627179</v>
+        <v>1.162331183734142</v>
       </c>
       <c r="Q2">
         <v>0.0539</v>
       </c>
       <c r="R2">
-        <v>0.176134257522376</v>
+        <v>0.1761342875078372</v>
       </c>
       <c r="S2">
-        <v>0.9979706319373389</v>
+        <v>1.000700311934588</v>
       </c>
       <c r="T2">
-        <v>1.004363503972236</v>
+        <v>1.001613830214347</v>
       </c>
       <c r="U2">
-        <v>3046.332719570178</v>
+        <v>3046.332499562711</v>
       </c>
       <c r="V2" t="s">
         <v>57</v>
@@ -887,55 +887,55 @@
         <v>34</v>
       </c>
       <c r="C3">
-        <v>1.000361813494442</v>
+        <v>1.000361813498088</v>
       </c>
       <c r="D3">
-        <v>330.3581063257659</v>
+        <v>330.3581063245617</v>
       </c>
       <c r="E3">
-        <v>1448.51774904885</v>
+        <v>1448.517749048326</v>
       </c>
       <c r="F3">
-        <v>1118.159642723084</v>
+        <v>1118.159642723764</v>
       </c>
       <c r="G3">
-        <v>213799.9609598223</v>
+        <v>213799.9636485063</v>
       </c>
       <c r="H3">
-        <v>48424.24286869316</v>
+        <v>48424.25939291456</v>
       </c>
       <c r="I3">
-        <v>3050.191976563085</v>
+        <v>3050.191836892714</v>
       </c>
       <c r="J3">
-        <v>553.7731528447774</v>
+        <v>553.7735900542677</v>
       </c>
       <c r="K3">
-        <v>1.48090255494528</v>
+        <v>1.480902597339079</v>
       </c>
       <c r="M3">
-        <v>1</v>
+        <v>0.123</v>
       </c>
       <c r="N3">
-        <v>1.915784197947801E-11</v>
+        <v>1.852173969751902E-11</v>
       </c>
       <c r="O3">
-        <v>0.9027261206850676</v>
+        <v>0.9027261388302016</v>
       </c>
       <c r="Q3">
-        <v>0.0772</v>
+        <v>0.07729999999999999</v>
       </c>
       <c r="R3">
-        <v>0.411162486683227</v>
+        <v>0.4111632472433012</v>
       </c>
       <c r="S3">
-        <v>0.9971105311931019</v>
+        <v>0.9997556499051803</v>
       </c>
       <c r="T3">
-        <v>1.003634368096894</v>
+        <v>1.000968712585147</v>
       </c>
       <c r="U3">
-        <v>3603.965129407862</v>
+        <v>3603.965426946982</v>
       </c>
       <c r="V3" t="s">
         <v>58</v>
@@ -967,55 +967,55 @@
         <v>35</v>
       </c>
       <c r="C4">
-        <v>1.001203534798631</v>
+        <v>1.001203543382377</v>
       </c>
       <c r="D4">
-        <v>330.0803711336287</v>
+        <v>330.0803683037084</v>
       </c>
       <c r="E4">
-        <v>1448.044888481254</v>
+        <v>1448.044885635041</v>
       </c>
       <c r="F4">
-        <v>1117.964517347625</v>
+        <v>1117.964517331332</v>
       </c>
       <c r="G4">
-        <v>200969.205816166</v>
+        <v>200969.2458278779</v>
       </c>
       <c r="H4">
-        <v>39896.70150131476</v>
+        <v>39896.69775952639</v>
       </c>
       <c r="I4">
-        <v>1674.819918540171</v>
+        <v>1674.778559078925</v>
       </c>
       <c r="J4">
-        <v>426.3044034446668</v>
+        <v>426.3043660926456</v>
       </c>
       <c r="K4">
-        <v>1.427475645258929</v>
+        <v>1.427484916621582</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>0.06279999999999999</v>
       </c>
       <c r="N4">
-        <v>4.792209573611927E-09</v>
+        <v>9.609033124746702E-09</v>
       </c>
       <c r="O4">
-        <v>1.128324226668517</v>
+        <v>1.128324366626255</v>
       </c>
       <c r="Q4">
         <v>0.0435</v>
       </c>
       <c r="R4">
-        <v>0.276485214711268</v>
+        <v>0.2764848457030177</v>
       </c>
       <c r="S4">
-        <v>0.9980483533706483</v>
+        <v>1.000881216811143</v>
       </c>
       <c r="T4">
-        <v>1.004378728766902</v>
+        <v>1.001526077626381</v>
       </c>
       <c r="U4">
-        <v>2101.124321984837</v>
+        <v>2101.08292517157</v>
       </c>
       <c r="V4" t="s">
         <v>59</v>
@@ -1047,55 +1047,55 @@
         <v>36</v>
       </c>
       <c r="C5">
-        <v>1.000463255801072</v>
+        <v>1.000463255777369</v>
       </c>
       <c r="D5">
-        <v>330.3246095550196</v>
+        <v>330.3246095628458</v>
       </c>
       <c r="E5">
-        <v>1448.386875299098</v>
+        <v>1448.386875308901</v>
       </c>
       <c r="F5">
-        <v>1118.062265744079</v>
+        <v>1118.062265746055</v>
       </c>
       <c r="G5">
-        <v>215030.7260549405</v>
+        <v>215030.7284951554</v>
       </c>
       <c r="H5">
-        <v>60122.56928737904</v>
+        <v>60122.5748071362</v>
       </c>
       <c r="I5">
-        <v>3010.880690886481</v>
+        <v>3010.880590751673</v>
       </c>
       <c r="J5">
-        <v>702.6382790976133</v>
+        <v>702.6384201881237</v>
       </c>
       <c r="K5">
-        <v>1.519435113097521</v>
+        <v>1.519435144852225</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>0.118</v>
       </c>
       <c r="N5">
-        <v>8.906685944332082E-10</v>
+        <v>8.906612669612457E-10</v>
       </c>
       <c r="O5">
-        <v>0.9027261208994443</v>
+        <v>0.9027261390496323</v>
       </c>
       <c r="Q5">
         <v>0.0519</v>
       </c>
       <c r="R5">
-        <v>0.4665655453707216</v>
+        <v>0.466565769070456</v>
       </c>
       <c r="S5">
-        <v>0.9972874504303466</v>
+        <v>0.9999489394960444</v>
       </c>
       <c r="T5">
-        <v>1.003659352131677</v>
+        <v>1.000978101400445</v>
       </c>
       <c r="U5">
-        <v>3713.518969984095</v>
+        <v>3713.519010939797</v>
       </c>
       <c r="V5" t="s">
         <v>60</v>
@@ -1127,55 +1127,55 @@
         <v>37</v>
       </c>
       <c r="C6">
-        <v>1.001018714221222</v>
+        <v>1.001018714199595</v>
       </c>
       <c r="D6">
-        <v>330.1413146943407</v>
+        <v>330.1413147014737</v>
       </c>
       <c r="E6">
-        <v>1448.136827523939</v>
+        <v>1448.136827525423</v>
       </c>
       <c r="F6">
-        <v>1117.995512829599</v>
+        <v>1117.99551282395</v>
       </c>
       <c r="G6">
-        <v>186271.0370431452</v>
+        <v>186271.0370859129</v>
       </c>
       <c r="H6">
-        <v>24002.35235459549</v>
+        <v>24002.34781785569</v>
       </c>
       <c r="I6">
-        <v>1314.688715120177</v>
+        <v>1314.688714041644</v>
       </c>
       <c r="J6">
-        <v>258.3647629723327</v>
+        <v>258.3645862895871</v>
       </c>
       <c r="K6">
-        <v>1.141979167200063</v>
+        <v>1.141979167462437</v>
       </c>
       <c r="M6">
-        <v>1</v>
+        <v>0.0501</v>
       </c>
       <c r="N6">
-        <v>0.4531543931906853</v>
+        <v>0.4531543951869683</v>
       </c>
       <c r="O6">
-        <v>1.075488560242321</v>
+        <v>1.075489068267882</v>
       </c>
       <c r="Q6">
         <v>0.0385</v>
       </c>
       <c r="R6">
-        <v>0.4146439925578138</v>
+        <v>0.4146431262716482</v>
       </c>
       <c r="S6">
-        <v>0.9978797610344818</v>
+        <v>1.000750142958378</v>
       </c>
       <c r="T6">
-        <v>1.004177477648039</v>
+        <v>1.001287429632395</v>
       </c>
       <c r="U6">
-        <v>1573.05347809251</v>
+        <v>1573.053300331231</v>
       </c>
       <c r="V6" t="s">
         <v>61</v>
@@ -1207,55 +1207,55 @@
         <v>38</v>
       </c>
       <c r="C7">
-        <v>1.000416166787789</v>
+        <v>1.00041616701041</v>
       </c>
       <c r="D7">
-        <v>330.3401577443067</v>
+        <v>330.3401576707965</v>
       </c>
       <c r="E7">
-        <v>1448.321952735371</v>
+        <v>1448.321952666135</v>
       </c>
       <c r="F7">
-        <v>1117.981794991064</v>
+        <v>1117.981794995339</v>
       </c>
       <c r="G7">
-        <v>220569.35749501</v>
+        <v>220569.3538159321</v>
       </c>
       <c r="H7">
-        <v>55930.85218171887</v>
+        <v>55930.85232523726</v>
       </c>
       <c r="I7">
-        <v>3180.623084596167</v>
+        <v>3180.623190413022</v>
       </c>
       <c r="J7">
-        <v>610.0843760544406</v>
+        <v>610.084370817436</v>
       </c>
       <c r="K7">
-        <v>1.552059543639453</v>
+        <v>1.552059506220811</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>0.123</v>
       </c>
       <c r="N7">
-        <v>2.210014393710935E-10</v>
+        <v>2.194725512438822E-10</v>
       </c>
       <c r="O7">
-        <v>1.093966515980028</v>
+        <v>1.093966507950459</v>
       </c>
       <c r="Q7">
         <v>0.0412</v>
       </c>
       <c r="R7">
-        <v>0.2568146536385955</v>
+        <v>0.2568146645005008</v>
       </c>
       <c r="S7">
-        <v>0.9972728598741181</v>
+        <v>0.9999191438069017</v>
       </c>
       <c r="T7">
-        <v>1.003579351147662</v>
+        <v>1.000913684563723</v>
       </c>
       <c r="U7">
-        <v>3790.707460650608</v>
+        <v>3790.707561230458</v>
       </c>
       <c r="V7" t="s">
         <v>62</v>
@@ -1287,55 +1287,55 @@
         <v>39</v>
       </c>
       <c r="C8">
-        <v>1.000438239106007</v>
+        <v>1.000438239082287</v>
       </c>
       <c r="D8">
-        <v>330.3328695651899</v>
+        <v>330.332869573022</v>
       </c>
       <c r="E8">
-        <v>1448.280386527096</v>
+        <v>1448.280386519248</v>
       </c>
       <c r="F8">
-        <v>1117.947516961906</v>
+        <v>1117.947516946226</v>
       </c>
       <c r="G8">
-        <v>194207.0685325385</v>
+        <v>194207.0712909518</v>
       </c>
       <c r="H8">
-        <v>38833.8509434377</v>
+        <v>38833.85284872806</v>
       </c>
       <c r="I8">
-        <v>1145.338090774124</v>
+        <v>1145.337883325554</v>
       </c>
       <c r="J8">
-        <v>421.7608218178106</v>
+        <v>421.7609188053179</v>
       </c>
       <c r="K8">
-        <v>1.416068662724578</v>
+        <v>1.416068707119019</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>0.0426</v>
       </c>
       <c r="N8">
-        <v>3.33066907387547E-15</v>
+        <v>1.942890293094024E-15</v>
       </c>
       <c r="O8">
-        <v>1.163611001704287</v>
+        <v>1.163610843400291</v>
       </c>
       <c r="Q8">
         <v>0.0438</v>
       </c>
       <c r="R8">
-        <v>0.2479657983611165</v>
+        <v>0.2479660788814572</v>
       </c>
       <c r="S8">
-        <v>0.9972869688752181</v>
+        <v>1.000176638528638</v>
       </c>
       <c r="T8">
-        <v>1.003609487502918</v>
+        <v>1.000699976517265</v>
       </c>
       <c r="U8">
-        <v>1567.098912591935</v>
+        <v>1567.098802130872</v>
       </c>
       <c r="V8" t="s">
         <v>63</v>
@@ -1367,55 +1367,55 @@
         <v>40</v>
       </c>
       <c r="C9">
-        <v>1.00024648209389</v>
+        <v>1.000246482117391</v>
       </c>
       <c r="D9">
-        <v>330.3961976000351</v>
+        <v>330.3961975922723</v>
       </c>
       <c r="E9">
-        <v>1448.539554282233</v>
+        <v>1448.53955427802</v>
       </c>
       <c r="F9">
-        <v>1118.143356682198</v>
+        <v>1118.143356685748</v>
       </c>
       <c r="G9">
-        <v>186360.9110065502</v>
+        <v>186360.9110493576</v>
       </c>
       <c r="H9">
-        <v>38526.15320144006</v>
+        <v>38526.15401897299</v>
       </c>
       <c r="I9">
-        <v>828.9340383794042</v>
+        <v>828.9340760286397</v>
       </c>
       <c r="J9">
-        <v>468.0145413567935</v>
+        <v>468.0145736862395</v>
       </c>
       <c r="K9">
-        <v>1.252845522224083</v>
+        <v>1.252845532945373</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>0.0483</v>
       </c>
       <c r="N9">
-        <v>0.1398524157712187</v>
+        <v>0.1398523776759204</v>
       </c>
       <c r="O9">
-        <v>0.9027261219529328</v>
+        <v>0.9027261400052951</v>
       </c>
       <c r="Q9">
         <v>0.07580000000000001</v>
       </c>
       <c r="R9">
-        <v>0.4504061814775351</v>
+        <v>0.4504062276145017</v>
       </c>
       <c r="S9">
-        <v>0.9970001591066461</v>
+        <v>0.999870920951148</v>
       </c>
       <c r="T9">
-        <v>1.003514014786304</v>
+        <v>1.000622325518441</v>
       </c>
       <c r="U9">
-        <v>1296.948579736198</v>
+        <v>1296.948649714879</v>
       </c>
       <c r="V9" t="s">
         <v>64</v>
@@ -1447,55 +1447,55 @@
         <v>41</v>
       </c>
       <c r="C10">
-        <v>1.000147305927082</v>
+        <v>1.000147305945619</v>
       </c>
       <c r="D10">
-        <v>330.4289602023155</v>
+        <v>330.4289601961912</v>
       </c>
       <c r="E10">
-        <v>1448.664947542881</v>
+        <v>1448.664947542898</v>
       </c>
       <c r="F10">
-        <v>1118.235987340566</v>
+        <v>1118.235987346707</v>
       </c>
       <c r="G10">
-        <v>186387.0034523646</v>
+        <v>186387.003495457</v>
       </c>
       <c r="H10">
-        <v>33046.55718231014</v>
+        <v>33046.55639200337</v>
       </c>
       <c r="I10">
-        <v>1105.609598676268</v>
+        <v>1105.609592455505</v>
       </c>
       <c r="J10">
-        <v>423.7891519862713</v>
+        <v>423.7891398537781</v>
       </c>
       <c r="K10">
-        <v>1.141979169116186</v>
+        <v>1.141979169388337</v>
       </c>
       <c r="M10">
-        <v>1</v>
+        <v>0.0547</v>
       </c>
       <c r="N10">
-        <v>0.2518075144887891</v>
+        <v>0.251807518047264</v>
       </c>
       <c r="O10">
-        <v>0.9027261206935806</v>
+        <v>0.9027261388435424</v>
       </c>
       <c r="Q10">
         <v>0.0815</v>
       </c>
       <c r="R10">
-        <v>0.3611504323540247</v>
+        <v>0.3611503616556817</v>
       </c>
       <c r="S10">
-        <v>0.9968844848664735</v>
+        <v>0.9997352236106604</v>
       </c>
       <c r="T10">
-        <v>1.003431555669575</v>
+        <v>1.000559728134313</v>
       </c>
       <c r="U10">
-        <v>1529.398750662539</v>
+        <v>1529.398732309284</v>
       </c>
       <c r="V10" t="s">
         <v>65</v>
@@ -1527,55 +1527,46 @@
         <v>42</v>
       </c>
       <c r="C11">
-        <v>1.000270190366446</v>
+        <v>1.000270190506009</v>
       </c>
       <c r="D11">
-        <v>330.3883665927935</v>
+        <v>330.3883665466963</v>
       </c>
       <c r="E11">
-        <v>1448.599158244529</v>
+        <v>1448.599158244362</v>
       </c>
       <c r="F11">
-        <v>1118.210791651736</v>
+        <v>1118.210791697665</v>
       </c>
       <c r="G11">
-        <v>186450.7849793156</v>
+        <v>186450.7850221031</v>
       </c>
       <c r="H11">
-        <v>30951.41914779498</v>
+        <v>30951.40903091468</v>
       </c>
       <c r="I11">
-        <v>1429.250193826431</v>
+        <v>1429.250186569565</v>
       </c>
       <c r="J11">
-        <v>394.7254015058338</v>
+        <v>394.7250319657187</v>
       </c>
       <c r="K11">
-        <v>1.141979167392954</v>
+        <v>1.141979167654315</v>
       </c>
       <c r="M11">
-        <v>1</v>
+        <v>0.0601</v>
       </c>
       <c r="N11">
-        <v>0.3278108641366846</v>
+        <v>0.3278108681134252</v>
       </c>
       <c r="O11">
-        <v>0.9027261206631648</v>
-      </c>
-      <c r="Q11">
-        <v>0.0842</v>
+        <v>0.9027261388131658</v>
       </c>
       <c r="R11">
-        <v>0.4177024994537846</v>
-      </c>
-      <c r="S11">
-        <v>0.9969984476954228</v>
-      </c>
-      <c r="T11">
-        <v>1.003563476787982</v>
+        <v>0.4177017271165545</v>
       </c>
       <c r="U11">
-        <v>1823.975595332265</v>
+        <v>1823.975218535284</v>
       </c>
       <c r="V11" t="s">
         <v>66</v>
@@ -1607,55 +1598,55 @@
         <v>43</v>
       </c>
       <c r="C12">
-        <v>1.000301696346043</v>
+        <v>1.00030169634916</v>
       </c>
       <c r="D12">
-        <v>330.3779605231298</v>
+        <v>330.3779605221002</v>
       </c>
       <c r="E12">
-        <v>1448.490883371716</v>
+        <v>1448.490883375149</v>
       </c>
       <c r="F12">
-        <v>1118.112922848587</v>
+        <v>1118.112922853049</v>
       </c>
       <c r="G12">
-        <v>186540.6589344398</v>
+        <v>186540.65897731</v>
       </c>
       <c r="H12">
-        <v>27273.75752056472</v>
+        <v>27273.7582690038</v>
       </c>
       <c r="I12">
-        <v>1662.100498347156</v>
+        <v>1662.100545722574</v>
       </c>
       <c r="J12">
-        <v>328.5295446550987</v>
+        <v>328.5295625388171</v>
       </c>
       <c r="K12">
-        <v>1.141979167272578</v>
+        <v>1.141979167536175</v>
       </c>
       <c r="M12">
-        <v>1</v>
+        <v>0.0668</v>
       </c>
       <c r="N12">
-        <v>0.4217492032346443</v>
+        <v>0.421749186980255</v>
       </c>
       <c r="O12">
-        <v>0.9027261208949983</v>
+        <v>0.9027261390646698</v>
       </c>
       <c r="Q12">
         <v>0.07149999999999999</v>
       </c>
       <c r="R12">
-        <v>0.5131536500483289</v>
+        <v>0.5131536999122317</v>
       </c>
       <c r="S12">
-        <v>0.9970679506463426</v>
+        <v>0.9998831338119145</v>
       </c>
       <c r="T12">
-        <v>1.003556486021084</v>
+        <v>1.000720609463311</v>
       </c>
       <c r="U12">
-        <v>1990.630043002255</v>
+        <v>1990.630108261391</v>
       </c>
       <c r="V12" t="s">
         <v>67</v>
@@ -1687,55 +1678,55 @@
         <v>44</v>
       </c>
       <c r="C13">
-        <v>1.000311914702563</v>
+        <v>1.000311914704606</v>
       </c>
       <c r="D13">
-        <v>330.3745856560136</v>
+        <v>330.3745856553387</v>
       </c>
       <c r="E13">
-        <v>1448.481722009104</v>
+        <v>1448.481722002183</v>
       </c>
       <c r="F13">
-        <v>1118.107136353091</v>
+        <v>1118.107136346845</v>
       </c>
       <c r="G13">
-        <v>186569.6505394095</v>
+        <v>186569.6505802802</v>
       </c>
       <c r="H13">
-        <v>25867.15529077611</v>
+        <v>25867.15558655941</v>
       </c>
       <c r="I13">
-        <v>1317.132087621014</v>
+        <v>1317.132254412622</v>
       </c>
       <c r="J13">
-        <v>290.4045058866883</v>
+        <v>290.4045264903806</v>
       </c>
       <c r="K13">
-        <v>1.141979167181807</v>
+        <v>1.1419791674438</v>
       </c>
       <c r="M13">
-        <v>1</v>
+        <v>0.0551</v>
       </c>
       <c r="N13">
-        <v>0.4207614221269546</v>
+        <v>0.4207613632438872</v>
       </c>
       <c r="O13">
-        <v>0.9027261502758491</v>
+        <v>0.9027261678033187</v>
       </c>
       <c r="Q13">
-        <v>0.0721</v>
+        <v>0.0722</v>
       </c>
       <c r="R13">
-        <v>0.5655134927696559</v>
+        <v>0.5655134876580054</v>
       </c>
       <c r="S13">
-        <v>0.9970762980855795</v>
+        <v>0.9999266227826269</v>
       </c>
       <c r="T13">
-        <v>1.003568599515058</v>
+        <v>1.000697503662557</v>
       </c>
       <c r="U13">
-        <v>1607.536593507702</v>
+        <v>1607.536780903003</v>
       </c>
       <c r="V13" t="s">
         <v>68</v>
@@ -1767,55 +1758,55 @@
         <v>45</v>
       </c>
       <c r="C14">
-        <v>1.000362202375852</v>
+        <v>1.00036220236927</v>
       </c>
       <c r="D14">
-        <v>330.357977902155</v>
+        <v>330.3579779043287</v>
       </c>
       <c r="E14">
-        <v>1448.452336783721</v>
+        <v>1448.452336788121</v>
       </c>
       <c r="F14">
-        <v>1118.094358881566</v>
+        <v>1118.094358883792</v>
       </c>
       <c r="G14">
-        <v>186355.1127000043</v>
+        <v>186355.1127367161</v>
       </c>
       <c r="H14">
-        <v>32616.5270377246</v>
+        <v>32616.52663691467</v>
       </c>
       <c r="I14">
-        <v>1013.89637622947</v>
+        <v>1013.896497104844</v>
       </c>
       <c r="J14">
-        <v>363.0311670146453</v>
+        <v>363.0311617399789</v>
       </c>
       <c r="K14">
-        <v>1.33855085069186</v>
+        <v>1.338550823995842</v>
       </c>
       <c r="M14">
-        <v>1</v>
+        <v>0.0422</v>
       </c>
       <c r="N14">
-        <v>0.01408050141126937</v>
+        <v>0.01408058457090111</v>
       </c>
       <c r="O14">
-        <v>0.9027261241604353</v>
+        <v>0.9027261423064551</v>
       </c>
       <c r="Q14">
         <v>0.0727</v>
       </c>
       <c r="R14">
-        <v>0.6199512808543294</v>
+        <v>0.6199512472726596</v>
       </c>
       <c r="S14">
-        <v>0.9971244558242027</v>
+        <v>1.00001439283712</v>
       </c>
       <c r="T14">
-        <v>1.003621043892622</v>
+        <v>1.000710253925056</v>
       </c>
       <c r="U14">
-        <v>1376.927543244116</v>
+        <v>1376.927658844823</v>
       </c>
       <c r="V14" t="s">
         <v>69</v>
@@ -1847,55 +1838,55 @@
         <v>46</v>
       </c>
       <c r="C15">
-        <v>1.00036934254286</v>
+        <v>1.00036934255411</v>
       </c>
       <c r="D15">
-        <v>330.3556199619079</v>
+        <v>330.3556199581928</v>
       </c>
       <c r="E15">
-        <v>1448.455617604829</v>
+        <v>1448.455617604647</v>
       </c>
       <c r="F15">
-        <v>1118.099997642921</v>
+        <v>1118.099997646454</v>
       </c>
       <c r="G15">
-        <v>186430.4908492587</v>
+        <v>186430.4908920626</v>
       </c>
       <c r="H15">
-        <v>29027.30056266392</v>
+        <v>29027.30126877719</v>
       </c>
       <c r="I15">
-        <v>656.2867677972048</v>
+        <v>656.2867711664837</v>
       </c>
       <c r="J15">
-        <v>327.8017567846139</v>
+        <v>327.8017744931564</v>
       </c>
       <c r="K15">
-        <v>1.259297822883219</v>
+        <v>1.259297822713707</v>
       </c>
       <c r="M15">
-        <v>1</v>
+        <v>0.0363</v>
       </c>
       <c r="N15">
-        <v>0.1867712290852031</v>
+        <v>0.1867712293404011</v>
       </c>
       <c r="O15">
-        <v>0.9027261207291524</v>
+        <v>0.9027261388699297</v>
       </c>
       <c r="Q15">
         <v>0.07240000000000001</v>
       </c>
       <c r="R15">
-        <v>0.6027207671158803</v>
+        <v>0.6027208093626665</v>
       </c>
       <c r="S15">
-        <v>0.9971324524239552</v>
+        <v>1.000040289942471</v>
       </c>
       <c r="T15">
-        <v>1.003627316280687</v>
+        <v>1.000698611779541</v>
       </c>
       <c r="U15">
-        <v>984.0885245818188</v>
+        <v>984.0885456596401</v>
       </c>
       <c r="V15" t="s">
         <v>70</v>
@@ -1927,55 +1918,55 @@
         <v>47</v>
       </c>
       <c r="C16">
-        <v>1.000371021664416</v>
+        <v>1.000371021738635</v>
       </c>
       <c r="D16">
-        <v>330.3550654603973</v>
+        <v>330.355065435888</v>
       </c>
       <c r="E16">
-        <v>1448.225767632338</v>
+        <v>1448.225767607844</v>
       </c>
       <c r="F16">
-        <v>1117.87070217194</v>
+        <v>1117.870702171956</v>
       </c>
       <c r="G16">
-        <v>182383.2633362079</v>
+        <v>182383.2633780849</v>
       </c>
       <c r="H16">
-        <v>11320.38458994558</v>
+        <v>11320.38394366622</v>
       </c>
       <c r="I16">
-        <v>5790.470891502586</v>
+        <v>5790.471104345149</v>
       </c>
       <c r="J16">
-        <v>98.63445843819724</v>
+        <v>98.63443805366033</v>
       </c>
       <c r="K16">
-        <v>1.141979167183938</v>
+        <v>1.141979167446091</v>
       </c>
       <c r="M16">
-        <v>1</v>
+        <v>0.296</v>
       </c>
       <c r="N16">
-        <v>0.6629511109506141</v>
+        <v>0.6629511549204886</v>
       </c>
       <c r="O16">
-        <v>1.199585416023738</v>
+        <v>1.199585496130716</v>
       </c>
       <c r="Q16">
         <v>0.0468</v>
       </c>
       <c r="R16">
-        <v>0.1911858959757372</v>
+        <v>0.1911856595153736</v>
       </c>
       <c r="S16">
-        <v>0.9972111469183175</v>
+        <v>0.9993340413946579</v>
       </c>
       <c r="T16">
-        <v>1.003550985532054</v>
+        <v>1.001410156407763</v>
       </c>
       <c r="U16">
-        <v>5889.105349940783</v>
+        <v>5889.105542398809</v>
       </c>
       <c r="V16" t="s">
         <v>71</v>
@@ -2007,55 +1998,55 @@
         <v>48</v>
       </c>
       <c r="C17">
-        <v>1.000535458314477</v>
+        <v>1.000535458332032</v>
       </c>
       <c r="D17">
-        <v>330.3007720519595</v>
+        <v>330.3007720461642</v>
       </c>
       <c r="E17">
-        <v>1448.417168715479</v>
+        <v>1448.417168715858</v>
       </c>
       <c r="F17">
-        <v>1118.116396663519</v>
+        <v>1118.116396669694</v>
       </c>
       <c r="G17">
-        <v>186413.0958886306</v>
+        <v>186413.09593143</v>
       </c>
       <c r="H17">
-        <v>30486.38123383373</v>
+        <v>30486.38175421131</v>
       </c>
       <c r="I17">
-        <v>2156.754655965494</v>
+        <v>2156.7546652389</v>
       </c>
       <c r="J17">
-        <v>381.4914027986494</v>
+        <v>381.4914216414805</v>
       </c>
       <c r="K17">
-        <v>1.141979167182616</v>
+        <v>1.141979167444843</v>
       </c>
       <c r="M17">
-        <v>1</v>
+        <v>0.0867</v>
       </c>
       <c r="N17">
-        <v>0.4622756405401924</v>
+        <v>0.4622756384666743</v>
       </c>
       <c r="O17">
-        <v>0.902726130905902</v>
+        <v>0.9027261490307966</v>
       </c>
       <c r="Q17">
         <v>0.0746</v>
       </c>
       <c r="R17">
-        <v>0.435001925425629</v>
+        <v>0.4350019711907531</v>
       </c>
       <c r="S17">
-        <v>0.9972908737913516</v>
+        <v>1.000047092546422</v>
       </c>
       <c r="T17">
-        <v>1.003801223599185</v>
+        <v>1.001024301330504</v>
       </c>
       <c r="U17">
-        <v>2538.246058764143</v>
+        <v>2538.24608688038</v>
       </c>
       <c r="V17" t="s">
         <v>72</v>
@@ -2087,55 +2078,55 @@
         <v>49</v>
       </c>
       <c r="C18">
-        <v>1.00055619087701</v>
+        <v>1.000556190874924</v>
       </c>
       <c r="D18">
-        <v>330.2939278772158</v>
+        <v>330.2939278779045</v>
       </c>
       <c r="E18">
-        <v>1448.113652871835</v>
+        <v>1448.113652877449</v>
       </c>
       <c r="F18">
-        <v>1117.81972499462</v>
+        <v>1117.819724999545</v>
       </c>
       <c r="G18">
-        <v>200344.0491382822</v>
+        <v>200344.0520801816</v>
       </c>
       <c r="H18">
-        <v>50303.17365272983</v>
+        <v>50303.17424460821</v>
       </c>
       <c r="I18">
-        <v>1714.594770248772</v>
+        <v>1714.594604445124</v>
       </c>
       <c r="J18">
-        <v>406.4744128841609</v>
+        <v>406.474405060326</v>
       </c>
       <c r="K18">
-        <v>1.439798314273101</v>
+        <v>1.43979835641463</v>
       </c>
       <c r="M18">
-        <v>1</v>
+        <v>0.0625</v>
       </c>
       <c r="N18">
-        <v>1.054711873393899E-15</v>
+        <v>5.551115123125783E-17</v>
       </c>
       <c r="O18">
-        <v>1.200422405709341</v>
+        <v>1.200422403231633</v>
       </c>
       <c r="Q18">
         <v>0.0515</v>
       </c>
       <c r="R18">
-        <v>0.0729244837113307</v>
+        <v>0.07292451697210411</v>
       </c>
       <c r="S18">
-        <v>0.9973810004376927</v>
+        <v>1.000210970932738</v>
       </c>
       <c r="T18">
-        <v>1.003751662497999</v>
+        <v>1.000901649202729</v>
       </c>
       <c r="U18">
-        <v>2121.069183132933</v>
+        <v>2121.06900950545</v>
       </c>
       <c r="V18" t="s">
         <v>73</v>
@@ -2167,55 +2158,55 @@
         <v>50</v>
       </c>
       <c r="C19">
-        <v>1.000681852802551</v>
+        <v>1.000681852581197</v>
       </c>
       <c r="D19">
-        <v>330.2524507875139</v>
+        <v>330.2524508605668</v>
       </c>
       <c r="E19">
-        <v>1448.263367712914</v>
+        <v>1448.263367787069</v>
       </c>
       <c r="F19">
-        <v>1118.010916925401</v>
+        <v>1118.010916926503</v>
       </c>
       <c r="G19">
-        <v>152139.2250725761</v>
+        <v>152139.2251075071</v>
       </c>
       <c r="H19">
-        <v>9456.028274208178</v>
+        <v>9456.024033668889</v>
       </c>
       <c r="I19">
-        <v>5421.459122769232</v>
+        <v>5421.458247092383</v>
       </c>
       <c r="J19">
-        <v>106.7636281424743</v>
+        <v>106.763529144387</v>
       </c>
       <c r="K19">
-        <v>1.141979167180183</v>
+        <v>1.141979167442376</v>
       </c>
       <c r="M19">
-        <v>1</v>
+        <v>0.34</v>
       </c>
       <c r="N19">
-        <v>0.6885119096218369</v>
+        <v>0.6885116670249152</v>
       </c>
       <c r="O19">
-        <v>0.9027261215944098</v>
+        <v>0.9027261396975661</v>
       </c>
       <c r="Q19">
         <v>0.0335</v>
       </c>
       <c r="R19">
-        <v>0.5051636211789438</v>
+        <v>0.5051625107155401</v>
       </c>
       <c r="S19">
-        <v>0.9975600642316416</v>
+        <v>0.9995514069190642</v>
       </c>
       <c r="T19">
-        <v>1.00382324151179</v>
+        <v>1.001814858100234</v>
       </c>
       <c r="U19">
-        <v>5528.222750911706</v>
+        <v>5528.22177623677</v>
       </c>
       <c r="V19" t="s">
         <v>74</v>
@@ -2247,55 +2238,46 @@
         <v>51</v>
       </c>
       <c r="C20">
-        <v>1.000630374921711</v>
+        <v>1.000630374936423</v>
       </c>
       <c r="D20">
-        <v>330.2694407737615</v>
+        <v>330.2694407689057</v>
       </c>
       <c r="E20">
-        <v>1448.047774422983</v>
+        <v>1448.047774423588</v>
       </c>
       <c r="F20">
-        <v>1117.778333649222</v>
+        <v>1117.778333654682</v>
       </c>
       <c r="G20">
-        <v>186331.9194054448</v>
+        <v>186331.9194482264</v>
       </c>
       <c r="H20">
-        <v>35579.16529913127</v>
+        <v>35579.16565682116</v>
       </c>
       <c r="I20">
-        <v>561.36076968027</v>
+        <v>561.3607433435405</v>
       </c>
       <c r="J20">
-        <v>267.599698473585</v>
+        <v>267.5996978979044</v>
       </c>
       <c r="K20">
-        <v>1.297537966325334</v>
-      </c>
-      <c r="M20">
-        <v>1</v>
+        <v>1.297537970494297</v>
       </c>
       <c r="N20">
-        <v>0.08839205159122021</v>
+        <v>0.08839204760862956</v>
       </c>
       <c r="O20">
-        <v>1.208417566734038</v>
+        <v>1.208417558714716</v>
       </c>
       <c r="Q20">
         <v>0.0516</v>
       </c>
       <c r="R20">
-        <v>0.127712972274836</v>
-      </c>
-      <c r="S20">
-        <v>0.9974544133232257</v>
-      </c>
-      <c r="T20">
-        <v>1.003826626071997</v>
+        <v>0.1277130124282202</v>
       </c>
       <c r="U20">
-        <v>828.960468153855</v>
+        <v>828.9604412414449</v>
       </c>
       <c r="V20" t="s">
         <v>75</v>
@@ -2327,55 +2309,55 @@
         <v>52</v>
       </c>
       <c r="C21">
-        <v>1.000263383788661</v>
+        <v>1.000263383791196</v>
       </c>
       <c r="D21">
-        <v>330.3906148147648</v>
+        <v>330.3906148139276</v>
       </c>
       <c r="E21">
-        <v>1448.213848878997</v>
+        <v>1448.213848872356</v>
       </c>
       <c r="F21">
-        <v>1117.823234064233</v>
+        <v>1117.823234058429</v>
       </c>
       <c r="G21">
-        <v>186627.6337370296</v>
+        <v>186627.6337798873</v>
       </c>
       <c r="H21">
-        <v>13224.74906363996</v>
+        <v>13224.74888721644</v>
       </c>
       <c r="I21">
-        <v>5373.149648894418</v>
+        <v>5373.149605047305</v>
       </c>
       <c r="J21">
-        <v>108.0678067003399</v>
+        <v>108.0678044056355</v>
       </c>
       <c r="K21">
-        <v>1.141979167179674</v>
+        <v>1.141979167441874</v>
       </c>
       <c r="M21">
-        <v>1</v>
+        <v>0.262</v>
       </c>
       <c r="N21">
-        <v>0.6391208466052772</v>
+        <v>0.6391208342495018</v>
       </c>
       <c r="O21">
-        <v>1.205481308793426</v>
+        <v>1.205481319453178</v>
       </c>
       <c r="Q21">
         <v>0.0507</v>
       </c>
       <c r="R21">
-        <v>0.1880473159993193</v>
+        <v>0.1880472678343537</v>
       </c>
       <c r="S21">
-        <v>0.9970924552098444</v>
+        <v>0.9993175742208035</v>
       </c>
       <c r="T21">
-        <v>1.003454544926654</v>
+        <v>1.00121098539092</v>
       </c>
       <c r="U21">
-        <v>5481.217455594758</v>
+        <v>5481.217409452941</v>
       </c>
       <c r="V21" t="s">
         <v>76</v>
@@ -2407,55 +2389,55 @@
         <v>53</v>
       </c>
       <c r="C22">
-        <v>1.000668021787366</v>
+        <v>1.000668021784316</v>
       </c>
       <c r="D22">
-        <v>330.2570154648718</v>
+        <v>330.2570154658786</v>
       </c>
       <c r="E22">
-        <v>1448.195285159826</v>
+        <v>1448.195285160139</v>
       </c>
       <c r="F22">
-        <v>1117.938269694955</v>
+        <v>1117.93826969426</v>
       </c>
       <c r="G22">
-        <v>186099.9865985308</v>
+        <v>186099.9866412664</v>
       </c>
       <c r="H22">
-        <v>36203.18176473047</v>
+        <v>36203.18186677825</v>
       </c>
       <c r="I22">
-        <v>753.4456714104759</v>
+        <v>753.44568551021</v>
       </c>
       <c r="J22">
-        <v>379.8123760767161</v>
+        <v>379.8123793709409</v>
       </c>
       <c r="K22">
-        <v>1.282288680429691</v>
+        <v>1.282288679812565</v>
       </c>
       <c r="M22">
-        <v>1</v>
+        <v>0.0364</v>
       </c>
       <c r="N22">
-        <v>0.1635922813973695</v>
+        <v>0.163592278331949</v>
       </c>
       <c r="O22">
-        <v>1.138490912677256</v>
+        <v>1.138490907794827</v>
       </c>
       <c r="Q22">
         <v>0.0432</v>
       </c>
       <c r="R22">
-        <v>0.1863666282629068</v>
+        <v>0.1863666397371903</v>
       </c>
       <c r="S22">
-        <v>0.9975171126372956</v>
+        <v>1.000426894489294</v>
       </c>
       <c r="T22">
-        <v>1.003838899895427</v>
+        <v>1.000909265342485</v>
       </c>
       <c r="U22">
-        <v>1133.258047487192</v>
+        <v>1133.258064881151</v>
       </c>
       <c r="V22" t="s">
         <v>77</v>
@@ -2487,55 +2469,55 @@
         <v>54</v>
       </c>
       <c r="C23">
-        <v>1.000562023332825</v>
+        <v>1.00056202348159</v>
       </c>
       <c r="D23">
-        <v>330.2920025345629</v>
+        <v>330.2920024854548</v>
       </c>
       <c r="E23">
-        <v>1448.272796830924</v>
+        <v>1448.272796779049</v>
       </c>
       <c r="F23">
-        <v>1117.980794296361</v>
+        <v>1117.980794293594</v>
       </c>
       <c r="G23">
-        <v>186076.7933157985</v>
+        <v>186076.7933585217</v>
       </c>
       <c r="H23">
-        <v>37778.88790202764</v>
+        <v>37778.88738363726</v>
       </c>
       <c r="I23">
-        <v>790.7865167282965</v>
+        <v>790.7865042224336</v>
       </c>
       <c r="J23">
-        <v>416.1813538616806</v>
+        <v>416.181344415356</v>
       </c>
       <c r="K23">
-        <v>1.288300389196726</v>
+        <v>1.288300385720027</v>
       </c>
       <c r="M23">
-        <v>1</v>
+        <v>0.0397</v>
       </c>
       <c r="N23">
-        <v>0.1529532626933061</v>
+        <v>0.1529532680360335</v>
       </c>
       <c r="O23">
-        <v>1.041122959572045</v>
+        <v>1.041122973626315</v>
       </c>
       <c r="Q23">
         <v>0.0364</v>
       </c>
       <c r="R23">
-        <v>0.3244427515578968</v>
+        <v>0.3244427057669688</v>
       </c>
       <c r="S23">
-        <v>0.9974322509588013</v>
+        <v>1.000331544905074</v>
       </c>
       <c r="T23">
-        <v>1.003711498916534</v>
+        <v>1.000792608288117</v>
       </c>
       <c r="U23">
-        <v>1206.967870589977</v>
+        <v>1206.96784863779</v>
       </c>
       <c r="V23" t="s">
         <v>78</v>
@@ -2567,55 +2549,55 @@
         <v>55</v>
       </c>
       <c r="C24">
-        <v>1.000537927102293</v>
+        <v>1.000537927145901</v>
       </c>
       <c r="D24">
-        <v>330.2999570478507</v>
+        <v>330.2999570334548</v>
       </c>
       <c r="E24">
-        <v>1448.115531665177</v>
+        <v>1448.115531664991</v>
       </c>
       <c r="F24">
-        <v>1117.815574617326</v>
+        <v>1117.815574631536</v>
       </c>
       <c r="G24">
-        <v>186381.2051307237</v>
+        <v>186381.2051735741</v>
       </c>
       <c r="H24">
-        <v>30474.35404577445</v>
+        <v>30474.35511942523</v>
       </c>
       <c r="I24">
-        <v>410.2874554441841</v>
+        <v>410.2874630550331</v>
       </c>
       <c r="J24">
-        <v>258.7019284998722</v>
+        <v>258.7019338771614</v>
       </c>
       <c r="K24">
-        <v>1.259763196957878</v>
+        <v>1.259763196385204</v>
       </c>
       <c r="M24">
-        <v>1</v>
+        <v>0.019</v>
       </c>
       <c r="N24">
-        <v>0.2030863546119819</v>
+        <v>0.2030863540825715</v>
       </c>
       <c r="O24">
-        <v>1.2317496883307</v>
+        <v>1.231749651244549</v>
       </c>
       <c r="Q24">
         <v>0.0514</v>
       </c>
       <c r="R24">
-        <v>0.1610662703701753</v>
+        <v>0.1610664062559768</v>
       </c>
       <c r="S24">
-        <v>0.9973631533940216</v>
+        <v>1.000324718337751</v>
       </c>
       <c r="T24">
-        <v>1.003732977024417</v>
+        <v>1.000751226859905</v>
       </c>
       <c r="U24">
-        <v>668.9893839440563</v>
+        <v>668.9893969321945</v>
       </c>
       <c r="V24" t="s">
         <v>79</v>
@@ -2647,55 +2629,55 @@
         <v>56</v>
       </c>
       <c r="C25">
-        <v>1.000098376758571</v>
+        <v>1.000098376761551</v>
       </c>
       <c r="D25">
-        <v>330.4451262262291</v>
+        <v>330.4451262252444</v>
       </c>
       <c r="E25">
-        <v>1448.553878748142</v>
+        <v>1448.553878750398</v>
       </c>
       <c r="F25">
-        <v>1118.108752521913</v>
+        <v>1118.108752525153</v>
       </c>
       <c r="G25">
-        <v>201929.4028167817</v>
+        <v>201929.4074392629</v>
       </c>
       <c r="H25">
-        <v>50278.44298087546</v>
+        <v>50278.44270802592</v>
       </c>
       <c r="I25">
-        <v>2318.611369834999</v>
+        <v>2318.611117523631</v>
       </c>
       <c r="J25">
-        <v>588.7805714505695</v>
+        <v>588.780574643259</v>
       </c>
       <c r="K25">
-        <v>1.401790285568223</v>
+        <v>1.401790346906763</v>
       </c>
       <c r="M25">
-        <v>1</v>
+        <v>0.096</v>
       </c>
       <c r="N25">
-        <v>1.039265895563801E-10</v>
+        <v>1.046821518357888E-10</v>
       </c>
       <c r="O25">
-        <v>0.9027261206633774</v>
+        <v>0.902726138813387</v>
       </c>
       <c r="Q25">
-        <v>0.0703</v>
+        <v>0.07190000000000001</v>
       </c>
       <c r="R25">
-        <v>0.4262674996854379</v>
+        <v>0.4262674795877546</v>
       </c>
       <c r="S25">
-        <v>0.9968695517689479</v>
+        <v>0.9995904823226196</v>
       </c>
       <c r="T25">
-        <v>1.003348185813224</v>
+        <v>1.000606787587745</v>
       </c>
       <c r="U25">
-        <v>2907.391941285568</v>
+        <v>2907.39169216689</v>
       </c>
       <c r="V25" t="s">
         <v>80</v>

</xml_diff>